<commit_message>
modified get review api
</commit_message>
<xml_diff>
--- a/04_API/capstone_API.xlsx
+++ b/04_API/capstone_API.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="68">
   <si>
     <t>Method</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>userName(string):UserName</t>
+  </si>
+  <si>
+    <t>/reviews/{property_id}</t>
   </si>
 </sst>
 </file>
@@ -510,7 +513,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A8"/>
+      <selection activeCell="C42" sqref="C42:C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1125,10 +1128,10 @@
         <v>23</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>9</v>
@@ -1245,28 +1248,30 @@
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="E30:E34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="E2:E6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A21"/>
@@ -1281,34 +1286,32 @@
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="E12:E14"/>
     <mergeCell ref="E15:E21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
     <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="E2:E6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="E40:E41"/>
     <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="E30:E34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>